<commit_message>
ajout cours de la semaine
</commit_message>
<xml_diff>
--- a/3BIN/BINV3140-1 Programmation - question spéciales/BINV3140-B ASP.NET/Roadmap.xlsx
+++ b/3BIN/BINV3140-1 Programmation - question spéciales/BINV3140-B ASP.NET/Roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents7\IPL\3BIN\BINV3140-1 Programmation - question spéciales\BINV3140-B ASP.NET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65CD725-15F8-4D20-8469-777821A92C3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497A8CB4-0DD1-42BF-B3D4-B95508787FDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -475,31 +475,31 @@
                   <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>160</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>160</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>160</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>160</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>160</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>160</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>160</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>160</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -937,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,10 +1015,12 @@
         <f>D3+C4</f>
         <v>240</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="5">
+        <v>90</v>
+      </c>
       <c r="F4" s="6">
         <f>F3+E4</f>
-        <v>160</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1038,7 +1040,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="6">
         <f t="shared" ref="F5:F12" si="1">F4+E5</f>
-        <v>160</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1058,7 +1060,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="6">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1078,7 +1080,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="6">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1098,7 +1100,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="6">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1118,7 +1120,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="6">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1138,7 +1140,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="6">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1158,7 +1160,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="6">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1178,7 +1180,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="6">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>